<commit_message>
Added changes for DCM'
</commit_message>
<xml_diff>
--- a/DCM_Motel6_Reporter.xlsx
+++ b/DCM_Motel6_Reporter.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9495" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Dimension" sheetId="1" r:id="rId1"/>
@@ -25,19 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
-  <si>
-    <t>dfa:advertiser</t>
-  </si>
-  <si>
-    <t>dfa:advertiserId</t>
-  </si>
-  <si>
-    <t>dfa:campaign</t>
-  </si>
-  <si>
-    <t>dfa:date</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t>dfa:placement</t>
   </si>
@@ -48,110 +36,164 @@
     <t>dfa:creativeId</t>
   </si>
   <si>
-    <t>dfa:flightBookedCost</t>
+    <t>dfa:clicks</t>
+  </si>
+  <si>
+    <t>dfa:richMediaExpansionTime</t>
+  </si>
+  <si>
+    <t>dfa:richMediaExpansions</t>
+  </si>
+  <si>
+    <t>dfa:richMediaFullScreenImpressions</t>
+  </si>
+  <si>
+    <t>dfa:richMediaFullScreenVideoCompletes</t>
+  </si>
+  <si>
+    <t>dfa:richMediaFullScreenVideoPlays</t>
+  </si>
+  <si>
+    <t>dfa:impressions</t>
+  </si>
+  <si>
+    <t>dfa:richMediaInteractiveImpressions</t>
+  </si>
+  <si>
+    <t>dfa:richMediaClicks</t>
+  </si>
+  <si>
+    <t>dfa:richMediaImpressions</t>
+  </si>
+  <si>
+    <t>dfa:richMediaDisplayTime</t>
+  </si>
+  <si>
+    <t>dfa:richMediaInteractionTime</t>
+  </si>
+  <si>
+    <t>dfa:richMediaInteractions</t>
+  </si>
+  <si>
+    <t>dfa:richMediaVideoCompanionClicks</t>
+  </si>
+  <si>
+    <t>dfa:richMediaVideoCompletions</t>
+  </si>
+  <si>
+    <t>dfa:richMediaVideoFirstQuartileCompletes</t>
+  </si>
+  <si>
+    <t>dfa:richMediaVideoFullScreens</t>
+  </si>
+  <si>
+    <t>dfa:richMediaVideoInteractions</t>
+  </si>
+  <si>
+    <t>dfa:richMediaVideoMutes</t>
+  </si>
+  <si>
+    <t>dfa:richMediaVideoPauses</t>
+  </si>
+  <si>
+    <t>dfa:richMediaVideoPlays</t>
+  </si>
+  <si>
+    <t>dfa:richMediaVideoReplays</t>
+  </si>
+  <si>
+    <t>dfa:richMediaVideoSkips</t>
+  </si>
+  <si>
+    <t>dfa:richMediaVideoStops</t>
+  </si>
+  <si>
+    <t>dfa:richMediaVideoThirdQuartileCompletes</t>
+  </si>
+  <si>
+    <t>dfa:richMediaVideoTrueViews</t>
+  </si>
+  <si>
+    <t>dfa:richMediaVideoUnmutes</t>
+  </si>
+  <si>
+    <t>dfa:richMediaVideoViews</t>
+  </si>
+  <si>
+    <t>dfa:city</t>
+  </si>
+  <si>
+    <t>dfa:appId</t>
+  </si>
+  <si>
+    <t>dfa:app</t>
+  </si>
+  <si>
+    <t>dfa:country</t>
+  </si>
+  <si>
+    <t>dfa:clickThroughUrl</t>
+  </si>
+  <si>
+    <t>dfa:creativeType</t>
+  </si>
+  <si>
+    <t>dfa:creative</t>
+  </si>
+  <si>
+    <t>dfa:dmaRegion</t>
+  </si>
+  <si>
+    <t>dfa:contentCategory</t>
+  </si>
+  <si>
+    <t>dfa:placementSize</t>
+  </si>
+  <si>
+    <t>dfa:placementStrategy</t>
+  </si>
+  <si>
+    <t>dfa:activeViewImpressionsVisible10Seconds</t>
+  </si>
+  <si>
+    <t>dfa:activeViewViewableImpressions</t>
+  </si>
+  <si>
+    <t>dfa:activeViewEligibleImpressions</t>
+  </si>
+  <si>
+    <t>dfa:activeViewMeasurableImpressions</t>
+  </si>
+  <si>
+    <t>dfa:activityClickThroughConversions</t>
+  </si>
+  <si>
+    <t>dfa:activityClickThroughRevenue</t>
+  </si>
+  <si>
+    <t>dfa:activityViewThroughConversions</t>
+  </si>
+  <si>
+    <t>dfa:activityViewThroughRevenue</t>
+  </si>
+  <si>
+    <t>dfa:totalConversionsRevenue</t>
+  </si>
+  <si>
+    <t>dfa:totalConversions</t>
   </si>
   <si>
     <t>dfa:richMediaBackupImages</t>
   </si>
   <si>
-    <t>dfa:bookedImpressions</t>
-  </si>
-  <si>
-    <t>dfa:clicks</t>
-  </si>
-  <si>
-    <t>dfa:richMediaExpansionTime</t>
-  </si>
-  <si>
-    <t>dfa:richMediaExpansions</t>
-  </si>
-  <si>
-    <t>dfa:richMediaFullScreenImpressions</t>
-  </si>
-  <si>
-    <t>dfa:richMediaFullScreenVideoCompletes</t>
-  </si>
-  <si>
-    <t>dfa:richMediaFullScreenVideoPlays</t>
-  </si>
-  <si>
-    <t>dfa:impressions</t>
-  </si>
-  <si>
-    <t>dfa:richMediaInteractiveImpressions</t>
-  </si>
-  <si>
-    <t>dfa:mediaCost</t>
-  </si>
-  <si>
-    <t>dfa:richMediaClicks</t>
-  </si>
-  <si>
-    <t>dfa:richMediaImpressions</t>
-  </si>
-  <si>
-    <t>dfa:richMediaDisplayTime</t>
-  </si>
-  <si>
-    <t>dfa:richMediaInteractionTime</t>
-  </si>
-  <si>
-    <t>dfa:richMediaInteractions</t>
-  </si>
-  <si>
-    <t>dfa:richMediaVideoCompanionClicks</t>
-  </si>
-  <si>
-    <t>dfa:richMediaVideoCompletions</t>
-  </si>
-  <si>
-    <t>dfa:richMediaVideoFirstQuartileCompletes</t>
-  </si>
-  <si>
-    <t>dfa:richMediaVideoFullScreens</t>
-  </si>
-  <si>
-    <t>dfa:richMediaVideoInteractions</t>
-  </si>
-  <si>
     <t>dfa:richMediaVideoMidpoints</t>
-  </si>
-  <si>
-    <t>dfa:richMediaVideoMutes</t>
-  </si>
-  <si>
-    <t>dfa:richMediaVideoPauses</t>
-  </si>
-  <si>
-    <t>dfa:richMediaVideoPlays</t>
-  </si>
-  <si>
-    <t>dfa:richMediaVideoReplays</t>
-  </si>
-  <si>
-    <t>dfa:richMediaVideoSkips</t>
-  </si>
-  <si>
-    <t>dfa:richMediaVideoStops</t>
-  </si>
-  <si>
-    <t>dfa:richMediaVideoThirdQuartileCompletes</t>
-  </si>
-  <si>
-    <t>dfa:richMediaVideoTrueViews</t>
-  </si>
-  <si>
-    <t>dfa:richMediaVideoUnmutes</t>
-  </si>
-  <si>
-    <t>dfa:richMediaVideoViews</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -162,6 +204,18 @@
     <font>
       <sz val="11"/>
       <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF212121"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -189,17 +243,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
+      <left style="medium">
+        <color rgb="FFDDDDDD"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
+      <right style="medium">
+        <color rgb="FFDDDDDD"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
+      <top style="medium">
+        <color rgb="FFDDDDDD"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
+      <bottom style="medium">
+        <color rgb="FFDDDDDD"/>
       </bottom>
       <diagonal/>
     </border>
@@ -207,15 +261,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="1"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -530,55 +597,85 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:A14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.85546875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="25.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>7</v>
+    <row r="13" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -588,10 +685,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A32"/>
+  <dimension ref="A1:A40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -599,164 +696,204 @@
     <col min="1" max="1" width="43" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+    <row r="7" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+    <row r="8" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+    <row r="23" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+    <row r="25" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+    <row r="26" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+    <row r="31" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+    <row r="32" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+    <row r="33" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+    <row r="34" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+    <row r="35" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
+    <row r="36" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+    <row r="37" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
+    <row r="38" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
+    <row r="39" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
+    <row r="40" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="5" t="s">
         <v>30</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
-        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>